<commit_message>
Atualização de bases das ligas, do dia: 2024-01-27 às 18-06
</commit_message>
<xml_diff>
--- a/Argentina Liga Profesional/Argentina Liga Profesional.xlsx
+++ b/Argentina Liga Profesional/Argentina Liga Profesional.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="41" uniqueCount="40">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="28" uniqueCount="28">
   <si>
     <t>id</t>
   </si>
@@ -61,12 +61,6 @@
     <t>oddA</t>
   </si>
   <si>
-    <t>Ah_op</t>
-  </si>
-  <si>
-    <t>oddAHH_op</t>
-  </si>
-  <si>
     <t>Ah</t>
   </si>
   <si>
@@ -76,15 +70,6 @@
     <t>oddAHA</t>
   </si>
   <si>
-    <t>AhOU_op</t>
-  </si>
-  <si>
-    <t>oddAHOver_op</t>
-  </si>
-  <si>
-    <t>oddAHUnder_op</t>
-  </si>
-  <si>
     <t>AhOU</t>
   </si>
   <si>
@@ -103,37 +88,16 @@
     <t>PLA</t>
   </si>
   <si>
-    <t>PLH_op</t>
-  </si>
-  <si>
-    <t>PLD_op</t>
-  </si>
-  <si>
-    <t>PLA_op</t>
-  </si>
-  <si>
     <t>PL_Ahh</t>
   </si>
   <si>
     <t>PL_Aha</t>
   </si>
   <si>
-    <t>PL_Ahh_op</t>
-  </si>
-  <si>
-    <t>PL_Aha_op</t>
-  </si>
-  <si>
     <t>PL_AhOver</t>
   </si>
   <si>
     <t>PL_AhUnder</t>
-  </si>
-  <si>
-    <t>PL_AhOver_op</t>
-  </si>
-  <si>
-    <t>PL_AhUnder_op</t>
   </si>
 </sst>
 </file>
@@ -491,13 +455,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="B1:AP1"/>
+  <dimension ref="B1:AC1"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="2:42">
+    <row r="1" spans="2:29">
       <c r="B1" s="1" t="s">
         <v>0</v>
       </c>
@@ -550,76 +514,37 @@
         <v>16</v>
       </c>
       <c r="S1" s="1" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="T1" s="1" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="U1" s="1" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="V1" s="1" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="W1" s="1" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="X1" s="1" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="Y1" s="1" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="Z1" s="1" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="AA1" s="1" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="AB1" s="1" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="AC1" s="1" t="s">
-        <v>26</v>
-      </c>
-      <c r="AD1" s="1" t="s">
         <v>27</v>
-      </c>
-      <c r="AE1" s="1" t="s">
-        <v>28</v>
-      </c>
-      <c r="AF1" s="1" t="s">
-        <v>29</v>
-      </c>
-      <c r="AG1" s="1" t="s">
-        <v>30</v>
-      </c>
-      <c r="AH1" s="1" t="s">
-        <v>31</v>
-      </c>
-      <c r="AI1" s="1" t="s">
-        <v>32</v>
-      </c>
-      <c r="AJ1" s="1" t="s">
-        <v>33</v>
-      </c>
-      <c r="AK1" s="1" t="s">
-        <v>34</v>
-      </c>
-      <c r="AL1" s="1" t="s">
-        <v>35</v>
-      </c>
-      <c r="AM1" s="1" t="s">
-        <v>36</v>
-      </c>
-      <c r="AN1" s="1" t="s">
-        <v>37</v>
-      </c>
-      <c r="AO1" s="1" t="s">
-        <v>38</v>
-      </c>
-      <c r="AP1" s="1" t="s">
-        <v>39</v>
       </c>
     </row>
   </sheetData>

</xml_diff>